<commit_message>
output in basic model
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fransdeboer/School/q3/aidm/aidm-assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC42D29C-C785-774E-A4BC-9D911014B5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0836E9-C759-3940-B451-463BABF3ADA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2849000C-4BE7-AE45-9E84-6022DF224E9D}"/>
   </bookViews>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Model</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
   <si>
     <t>Time 1</t>
   </si>
@@ -50,6 +47,15 @@
   </si>
   <si>
     <t>DNF</t>
+  </si>
+  <si>
+    <t>Gecode</t>
+  </si>
+  <si>
+    <t>Model 1</t>
+  </si>
+  <si>
+    <t>Model 2</t>
   </si>
 </sst>
 </file>
@@ -401,218 +407,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BBB967C-38B9-AF43-AA1D-66E1FF000DB0}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>379</v>
+      </c>
+      <c r="C3">
+        <v>425</v>
+      </c>
+      <c r="D3">
+        <v>290</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>260</v>
+      </c>
+      <c r="C4">
+        <v>373</v>
+      </c>
+      <c r="D4">
+        <v>506</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="B5">
+        <v>333</v>
+      </c>
+      <c r="C5">
+        <v>286</v>
+      </c>
+      <c r="D5">
         <v>379</v>
       </c>
-      <c r="C2">
-        <v>425</v>
-      </c>
-      <c r="D2">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>260</v>
-      </c>
-      <c r="C3">
-        <v>373</v>
-      </c>
-      <c r="D3">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="J5">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>333</v>
-      </c>
-      <c r="C4">
-        <v>286</v>
-      </c>
-      <c r="D4">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>346</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>410</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>402</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="J6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>320</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>325</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>323</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="J7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>236</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>236</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>233</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="J8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="J9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>359</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>315</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>423</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="J10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>698</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>737</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>590</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="J12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="J13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="J14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="J15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>357</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>344</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>285</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="J16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="J17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>330</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>628</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>1408</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="J18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="J19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="J20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="J21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added o to output of basic model
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fransdeboer/School/q3/aidm/aidm-assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0836E9-C759-3940-B451-463BABF3ADA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75030812-F141-1E41-B2D7-A9B9AE7D82BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2849000C-4BE7-AE45-9E84-6022DF224E9D}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2849000C-4BE7-AE45-9E84-6022DF224E9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
   <si>
     <t>Time 1</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Time 3</t>
   </si>
   <si>
-    <t>DNF</t>
-  </si>
-  <si>
     <t>Gecode</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>Model 2</t>
+  </si>
+  <si>
+    <t>COIN-BC</t>
   </si>
 </sst>
 </file>
@@ -410,22 +410,25 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -446,7 +449,7 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
         <v>0</v>
@@ -480,8 +483,14 @@
       <c r="D3">
         <v>290</v>
       </c>
+      <c r="F3">
+        <v>1460</v>
+      </c>
       <c r="J3">
         <v>1</v>
+      </c>
+      <c r="K3">
+        <v>480</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -497,8 +506,14 @@
       <c r="D4">
         <v>506</v>
       </c>
+      <c r="F4">
+        <v>16949</v>
+      </c>
       <c r="J4">
         <v>2</v>
+      </c>
+      <c r="K4">
+        <v>1230</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -514,6 +529,9 @@
       <c r="D5">
         <v>379</v>
       </c>
+      <c r="F5">
+        <v>23878</v>
+      </c>
       <c r="J5">
         <v>3</v>
       </c>
@@ -531,6 +549,9 @@
       <c r="D6">
         <v>402</v>
       </c>
+      <c r="F6">
+        <v>809</v>
+      </c>
       <c r="J6">
         <v>4</v>
       </c>
@@ -548,6 +569,9 @@
       <c r="D7">
         <v>323</v>
       </c>
+      <c r="F7">
+        <v>32214</v>
+      </c>
       <c r="J7">
         <v>5</v>
       </c>
@@ -565,6 +589,9 @@
       <c r="D8">
         <v>233</v>
       </c>
+      <c r="F8">
+        <v>621</v>
+      </c>
       <c r="J8">
         <v>6</v>
       </c>
@@ -573,6 +600,9 @@
       <c r="A9">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
       <c r="J9">
         <v>7</v>
       </c>
@@ -590,6 +620,9 @@
       <c r="D10">
         <v>423</v>
       </c>
+      <c r="F10">
+        <v>11844</v>
+      </c>
       <c r="J10">
         <v>8</v>
       </c>
@@ -598,8 +631,11 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
+      <c r="B11">
+        <v>1.29</v>
+      </c>
+      <c r="F11">
+        <v>4705</v>
       </c>
       <c r="J11">
         <v>9</v>
@@ -618,6 +654,9 @@
       <c r="D12">
         <v>590</v>
       </c>
+      <c r="F12">
+        <v>859</v>
+      </c>
       <c r="J12">
         <v>10</v>
       </c>
@@ -626,6 +665,9 @@
       <c r="A13">
         <v>11</v>
       </c>
+      <c r="B13">
+        <v>-1</v>
+      </c>
       <c r="J13">
         <v>11</v>
       </c>
@@ -634,6 +676,9 @@
       <c r="A14">
         <v>12</v>
       </c>
+      <c r="B14">
+        <v>-1</v>
+      </c>
       <c r="J14">
         <v>12</v>
       </c>
@@ -642,6 +687,9 @@
       <c r="A15">
         <v>13</v>
       </c>
+      <c r="B15">
+        <v>-1</v>
+      </c>
       <c r="J15">
         <v>13</v>
       </c>
@@ -659,6 +707,9 @@
       <c r="D16">
         <v>285</v>
       </c>
+      <c r="F16">
+        <v>15934</v>
+      </c>
       <c r="J16">
         <v>14</v>
       </c>
@@ -667,6 +718,9 @@
       <c r="A17">
         <v>15</v>
       </c>
+      <c r="B17">
+        <v>-1</v>
+      </c>
       <c r="J17">
         <v>15</v>
       </c>
@@ -684,6 +738,9 @@
       <c r="D18">
         <v>1408</v>
       </c>
+      <c r="F18">
+        <v>3872</v>
+      </c>
       <c r="J18">
         <v>16</v>
       </c>
@@ -692,6 +749,9 @@
       <c r="A19">
         <v>17</v>
       </c>
+      <c r="B19">
+        <v>-1</v>
+      </c>
       <c r="J19">
         <v>17</v>
       </c>
@@ -700,6 +760,9 @@
       <c r="A20">
         <v>18</v>
       </c>
+      <c r="B20">
+        <v>-1</v>
+      </c>
       <c r="J20">
         <v>18</v>
       </c>
@@ -708,6 +771,9 @@
       <c r="A21">
         <v>19</v>
       </c>
+      <c r="B21">
+        <v>-1</v>
+      </c>
       <c r="J21">
         <v>19</v>
       </c>
@@ -716,8 +782,8 @@
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>3</v>
+      <c r="B22">
+        <v>-1</v>
       </c>
       <c r="J22">
         <v>20</v>

</xml_diff>

<commit_message>
tried some domain constraints
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fransdeboer/School/q3/aidm/aidm-assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59535952-CCF4-AB4E-89F6-72DDBE2B38B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C4DD96-83F9-304D-8CEE-95FB9EC82958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2849000C-4BE7-AE45-9E84-6022DF224E9D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Time 1</t>
   </si>
@@ -50,6 +50,39 @@
   </si>
   <si>
     <t>COIN-BC</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Model 2 - COIN</t>
+  </si>
+  <si>
+    <t>Model 1- Gecode</t>
+  </si>
+  <si>
+    <t>Optimizing Model 1</t>
+  </si>
+  <si>
+    <t>--use-gecode</t>
+  </si>
+  <si>
+    <t>--shave</t>
+  </si>
+  <si>
+    <t>--sac</t>
+  </si>
+  <si>
+    <t>--shave --sac</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>--shave --sac --pre-passed 3</t>
+  </si>
+  <si>
+    <t>--free-search</t>
   </si>
 </sst>
 </file>
@@ -403,15 +436,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BBB967C-38B9-AF43-AA1D-66E1FF000DB0}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -424,8 +460,11 @@
       <c r="I1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -445,7 +484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -464,8 +503,14 @@
       <c r="I3">
         <v>11.596</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -484,8 +529,20 @@
       <c r="I4">
         <v>2.4700000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <v>9</v>
+      </c>
+      <c r="M4">
+        <v>47.95</v>
+      </c>
+      <c r="O4">
+        <v>9</v>
+      </c>
+      <c r="P4">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -504,8 +561,20 @@
       <c r="I5">
         <v>54.265000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>16</v>
+      </c>
+      <c r="M5">
+        <v>4.57</v>
+      </c>
+      <c r="O5">
+        <v>16</v>
+      </c>
+      <c r="P5">
+        <v>57.77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -525,7 +594,7 @@
         <v>1.8979999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -544,8 +613,14 @@
       <c r="I7">
         <v>1.284</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -564,8 +639,20 @@
       <c r="I8">
         <v>1.179</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>9</v>
+      </c>
+      <c r="M8">
+        <v>49.96</v>
+      </c>
+      <c r="O8">
+        <v>9</v>
+      </c>
+      <c r="P8">
+        <v>4.5199999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -584,8 +671,20 @@
       <c r="I9">
         <v>-1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <v>16</v>
+      </c>
+      <c r="M9">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="O9">
+        <v>16</v>
+      </c>
+      <c r="P9">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -605,7 +704,7 @@
         <v>5.1100000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -624,8 +723,11 @@
       <c r="I11">
         <v>16.331</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -644,8 +746,14 @@
       <c r="I12">
         <v>33.954000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>9</v>
+      </c>
+      <c r="M12">
+        <v>52.24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -665,8 +773,14 @@
       <c r="I13">
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <v>16</v>
+      </c>
+      <c r="M13">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -686,7 +800,7 @@
         <v>10.093</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -705,8 +819,11 @@
       <c r="I15">
         <v>21.302</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -725,8 +842,14 @@
       <c r="I16">
         <v>3.5550000000000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>9</v>
+      </c>
+      <c r="M16">
+        <v>51.61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -745,8 +868,14 @@
       <c r="I17">
         <v>-1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>16</v>
+      </c>
+      <c r="M17">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -766,7 +895,7 @@
         <v>6.9550000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -785,8 +914,11 @@
       <c r="I19">
         <v>5.5949999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -805,8 +937,14 @@
       <c r="I20">
         <v>-1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <v>9</v>
+      </c>
+      <c r="M20">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -825,8 +963,14 @@
       <c r="I21">
         <v>-1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <v>16</v>
+      </c>
+      <c r="M21">
+        <v>52.33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -845,6 +989,202 @@
       <c r="I22">
         <f>56*60+38</f>
         <v>3398</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
+      <c r="K26">
+        <v>6</v>
+      </c>
+      <c r="M26">
+        <v>7</v>
+      </c>
+      <c r="O26">
+        <v>8</v>
+      </c>
+      <c r="Q26">
+        <v>9</v>
+      </c>
+      <c r="S26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="E32">
+        <v>13</v>
+      </c>
+      <c r="G32">
+        <v>14</v>
+      </c>
+      <c r="I32">
+        <v>15</v>
+      </c>
+      <c r="K32">
+        <v>16</v>
+      </c>
+      <c r="M32">
+        <v>17</v>
+      </c>
+      <c r="O32">
+        <v>18</v>
+      </c>
+      <c r="Q32">
+        <v>19</v>
+      </c>
+      <c r="S32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="I38">
+        <v>5</v>
+      </c>
+      <c r="K38">
+        <v>6</v>
+      </c>
+      <c r="M38">
+        <v>7</v>
+      </c>
+      <c r="O38">
+        <v>8</v>
+      </c>
+      <c r="Q38">
+        <v>9</v>
+      </c>
+      <c r="S38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>1.19</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>1.83</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>11.91</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I39">
+        <v>5</v>
+      </c>
+      <c r="J39">
+        <v>1.67</v>
+      </c>
+      <c r="K39">
+        <v>2</v>
+      </c>
+      <c r="L39">
+        <v>0.65</v>
+      </c>
+      <c r="O39">
+        <v>11</v>
+      </c>
+      <c r="P39">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>2.41</v>
+      </c>
+      <c r="K40" t="s">
+        <v>5</v>
+      </c>
+      <c r="L40">
+        <v>10.87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <v>12</v>
+      </c>
+      <c r="E44">
+        <v>13</v>
+      </c>
+      <c r="G44">
+        <v>14</v>
+      </c>
+      <c r="I44">
+        <v>15</v>
+      </c>
+      <c r="K44">
+        <v>16</v>
+      </c>
+      <c r="M44">
+        <v>17</v>
+      </c>
+      <c r="O44">
+        <v>18</v>
+      </c>
+      <c r="Q44">
+        <v>19</v>
+      </c>
+      <c r="S44">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished statistics, started update on model 2 output
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fransdeboer/School/q3/aidm/aidm-assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766DDF4D-F2C9-9A4F-94BB-7CD92E6093E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9D6B9B-1FEB-4748-9B75-9110EFD4CA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2849000C-4BE7-AE45-9E84-6022DF224E9D}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2849000C-4BE7-AE45-9E84-6022DF224E9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Time 1</t>
   </si>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BBB967C-38B9-AF43-AA1D-66E1FF000DB0}">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="R46" sqref="R46"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1261,6 +1261,12 @@
       <c r="O33" t="s">
         <v>20</v>
       </c>
+      <c r="Q33" t="s">
+        <v>20</v>
+      </c>
+      <c r="S33" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -1397,7 +1403,7 @@
         <v>13</v>
       </c>
       <c r="T40">
-        <v>36000</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
final statistics and final model name
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fransdeboer/School/q3/aidm/aidm-assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9D6B9B-1FEB-4748-9B75-9110EFD4CA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D406C844-C7CE-BF46-A262-CF05F064DD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2849000C-4BE7-AE45-9E84-6022DF224E9D}"/>
   </bookViews>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BBB967C-38B9-AF43-AA1D-66E1FF000DB0}">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="S34" sqref="S34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>